<commit_message>
Atualização da lista de CSAP
</commit_message>
<xml_diff>
--- a/Bibliografia/MS/Lista de CSAP.xlsx
+++ b/Bibliografia/MS/Lista de CSAP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a8628a50772066/R/ICSAP/Bibliografia/MS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="311" documentId="11_FB52EA33A9503895B47D68A18B6C5A6365C60DC0" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0EAD68E2-ED3A-4C09-9971-15039CD45BA7}"/>
+  <xr:revisionPtr revIDLastSave="336" documentId="11_FB52EA33A9503895B47D68A18B6C5A6365C60DC0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD296E62-3CAF-4376-90C1-FF2DE3AE6987}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="336">
   <si>
     <t>LISTA DE CONDIÇÕES SENSÍVEIS À ATENÇÃO PRIMÁRIA</t>
   </si>
@@ -989,6 +989,60 @@
   </si>
   <si>
     <t>1992 - 1997</t>
+  </si>
+  <si>
+    <t>CID 9</t>
+  </si>
+  <si>
+    <t>033</t>
+  </si>
+  <si>
+    <t>032</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>072</t>
+  </si>
+  <si>
+    <t>056</t>
+  </si>
+  <si>
+    <t>055</t>
+  </si>
+  <si>
+    <t>060</t>
+  </si>
+  <si>
+    <t>0702, 0703</t>
+  </si>
+  <si>
+    <t>3200</t>
+  </si>
+  <si>
+    <t>3204</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>390, 391</t>
+  </si>
+  <si>
+    <t>090 a 099</t>
+  </si>
+  <si>
+    <t>084</t>
+  </si>
+  <si>
+    <t>1270</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1182,6 +1236,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1474,11 +1534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1486,17 +1546,18 @@
     <col min="1" max="1" width="30.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="54.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="14" style="21" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1506,9 +1567,12 @@
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="D2" s="20" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1517,153 +1581,204 @@
       <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
+      <c r="D3" s="21" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
+      <c r="D4" s="21" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
+      <c r="D5" s="21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
+      <c r="D6" s="21" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
+      <c r="D7" s="21" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="24"/>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
+      <c r="D8" s="21" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="24"/>
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
+      <c r="D9" s="21" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
+      <c r="D10" s="21" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
+      <c r="D11" s="21" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="24"/>
       <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
+      <c r="D12" s="21" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
+      <c r="D13" s="21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
+      <c r="D14" s="21" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="24"/>
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
+      <c r="D15" s="21" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
       <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
+      <c r="D16" s="21" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="24"/>
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
+      <c r="D17" s="21" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
       <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
+      <c r="D18" s="21" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="25"/>
       <c r="B19" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="D19" s="21" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1673,8 +1788,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="25"/>
       <c r="B21" s="9" t="s">
         <v>42</v>
       </c>
@@ -1682,7 +1797,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>44</v>
       </c>
@@ -1693,8 +1808,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+    <row r="23" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1704,8 +1819,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="25"/>
       <c r="B24" s="9" t="s">
         <v>50</v>
       </c>
@@ -1713,8 +1828,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -1724,8 +1839,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="24"/>
       <c r="B26" s="3" t="s">
         <v>55</v>
       </c>
@@ -1733,8 +1848,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="24"/>
       <c r="B27" s="3" t="s">
         <v>57</v>
       </c>
@@ -1742,8 +1857,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="24"/>
       <c r="B28" s="3" t="s">
         <v>59</v>
       </c>
@@ -1751,8 +1866,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="24"/>
       <c r="B29" s="3" t="s">
         <v>61</v>
       </c>
@@ -1760,8 +1875,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
       <c r="B30" s="3" t="s">
         <v>63</v>
       </c>
@@ -1769,8 +1884,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="23"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="25"/>
       <c r="B31" s="9" t="s">
         <v>65</v>
       </c>
@@ -1778,8 +1893,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
         <v>67</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -1790,7 +1905,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="22"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="3" t="s">
         <v>70</v>
       </c>
@@ -1799,7 +1914,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="22"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="3" t="s">
         <v>72</v>
       </c>
@@ -1808,7 +1923,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="22"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="3" t="s">
         <v>74</v>
       </c>
@@ -1817,7 +1932,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="23"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="9" t="s">
         <v>76</v>
       </c>
@@ -1837,7 +1952,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="23" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -1848,7 +1963,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="22"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="3" t="s">
         <v>83</v>
       </c>
@@ -1857,7 +1972,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="22"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="3" t="s">
         <v>85</v>
       </c>
@@ -1866,7 +1981,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="22"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="3" t="s">
         <v>87</v>
       </c>
@@ -1875,7 +1990,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="22"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="3" t="s">
         <v>89</v>
       </c>
@@ -1884,7 +1999,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="22"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="3" t="s">
         <v>91</v>
       </c>
@@ -1893,7 +2008,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="23"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="9" t="s">
         <v>93</v>
       </c>
@@ -1902,7 +2017,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="23" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -1913,7 +2028,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="23"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="9" t="s">
         <v>98</v>
       </c>
@@ -1933,7 +2048,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="23" t="s">
         <v>103</v>
       </c>
       <c r="B48" s="7" t="s">
@@ -1944,7 +2059,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="23"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="9" t="s">
         <v>105</v>
       </c>
@@ -1964,7 +2079,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="21" t="s">
+      <c r="A51" s="23" t="s">
         <v>109</v>
       </c>
       <c r="B51" s="7" t="s">
@@ -1975,7 +2090,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="22"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="3" t="s">
         <v>165</v>
       </c>
@@ -1984,7 +2099,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="23"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="9" t="s">
         <v>113</v>
       </c>
@@ -2004,7 +2119,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="23" t="s">
         <v>117</v>
       </c>
       <c r="B55" s="7" t="s">
@@ -2015,7 +2130,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="22"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="3" t="s">
         <v>120</v>
       </c>
@@ -2024,7 +2139,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="22"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="3" t="s">
         <v>122</v>
       </c>
@@ -2033,7 +2148,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="22"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="3" t="s">
         <v>124</v>
       </c>
@@ -2042,7 +2157,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="22"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="3" t="s">
         <v>126</v>
       </c>
@@ -2051,7 +2166,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="23"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="9" t="s">
         <v>128</v>
       </c>
@@ -2060,7 +2175,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="23" t="s">
         <v>130</v>
       </c>
       <c r="B61" s="7" t="s">
@@ -2071,7 +2186,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="22"/>
+      <c r="A62" s="24"/>
       <c r="B62" s="3" t="s">
         <v>133</v>
       </c>
@@ -2080,7 +2195,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="22"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="3" t="s">
         <v>135</v>
       </c>
@@ -2089,7 +2204,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="22"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="3" t="s">
         <v>137</v>
       </c>
@@ -2098,7 +2213,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="22"/>
+      <c r="A65" s="24"/>
       <c r="B65" s="3" t="s">
         <v>139</v>
       </c>
@@ -2107,7 +2222,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A66" s="23"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="9" t="s">
         <v>141</v>
       </c>
@@ -2116,7 +2231,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="21" t="s">
+      <c r="A67" s="23" t="s">
         <v>143</v>
       </c>
       <c r="B67" s="7" t="s">
@@ -2127,7 +2242,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="22"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="3" t="s">
         <v>146</v>
       </c>
@@ -2136,7 +2251,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="22"/>
+      <c r="A69" s="24"/>
       <c r="B69" s="3" t="s">
         <v>148</v>
       </c>
@@ -2145,7 +2260,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="22"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="3" t="s">
         <v>150</v>
       </c>
@@ -2154,7 +2269,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="22"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="3" t="s">
         <v>152</v>
       </c>
@@ -2163,7 +2278,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A72" s="23"/>
+      <c r="A72" s="25"/>
       <c r="B72" s="9" t="s">
         <v>154</v>
       </c>
@@ -2183,7 +2298,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="21" t="s">
+      <c r="A74" s="23" t="s">
         <v>158</v>
       </c>
       <c r="B74" s="7" t="s">
@@ -2194,7 +2309,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="22"/>
+      <c r="A75" s="24"/>
       <c r="B75" s="3" t="s">
         <v>161</v>
       </c>
@@ -2203,7 +2318,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="23"/>
+      <c r="A76" s="25"/>
       <c r="B76" s="9" t="s">
         <v>163</v>
       </c>
@@ -2230,6 +2345,9 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>